<commit_message>
Conduct S4 tests for Graphql
</commit_message>
<xml_diff>
--- a/Wyniki 3/Ostateczne wyniki/S2 - podsumowanie.xlsx
+++ b/Wyniki 3/Ostateczne wyniki/S2 - podsumowanie.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kacpe\OneDrive\Pulpit\Projekty\Praca magisterska\Wyniki 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kacpe\OneDrive\Pulpit\Projekty\Praca magisterska\Wyniki 3\Ostateczne wyniki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3ADC96-F643-4EA5-A007-207D2B580521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2988CC6-2F4F-49B7-9208-2BA52097F8F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25710" yWindow="-2340" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -905,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="G5:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>